<commit_message>
Trying to mess with weapons
</commit_message>
<xml_diff>
--- a/design documents/jRPG balance scratchsheet.xlsx
+++ b/design documents/jRPG balance scratchsheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Godot\jRPG-Attempt\design documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F16A535-4ECC-4E30-92CD-22244D912A34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89F9910A-605C-4747-8E26-5DEEF17DA54E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="5" activeTab="8" xr2:uid="{B20A1628-0B43-4A65-B110-26A0C753EEB6}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="5" activeTab="9" xr2:uid="{B20A1628-0B43-4A65-B110-26A0C753EEB6}"/>
   </bookViews>
   <sheets>
     <sheet name="Linear" sheetId="1" state="hidden" r:id="rId1"/>
@@ -21,7 +21,8 @@
     <sheet name="Stat Progression &amp; Growth Rates" sheetId="6" r:id="rId6"/>
     <sheet name="Stats (Old)" sheetId="7" state="hidden" r:id="rId7"/>
     <sheet name="Stats (New)" sheetId="9" r:id="rId8"/>
-    <sheet name="Archetypes" sheetId="8" r:id="rId9"/>
+    <sheet name="Archetypes Scratchsheet" sheetId="8" r:id="rId9"/>
+    <sheet name="What Is A Weapon" sheetId="10" r:id="rId10"/>
   </sheets>
   <definedNames>
     <definedName name="StatsByGrowthRateAndLevel">'Stat Progression &amp; Growth Rates'!$F$2:$Q$103</definedName>
@@ -47,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="99">
   <si>
     <t xml:space="preserve">LOG of </t>
   </si>
@@ -285,6 +286,66 @@
   <si>
     <t>White Mage</t>
   </si>
+  <si>
+    <t>STATS</t>
+  </si>
+  <si>
+    <t>TOTAL GROWTH</t>
+  </si>
+  <si>
+    <t>Stats At Level</t>
+  </si>
+  <si>
+    <t>Weapons have a Rarity and a Level.</t>
+  </si>
+  <si>
+    <t>At baseline, a weapon's damage is equal to STR of a character with (Rarity) Growth, at that Level.</t>
+  </si>
+  <si>
+    <t>Thus, a character's total attack damage is something like STR + Weapon Damage.</t>
+  </si>
+  <si>
+    <t>Maybe reduce it by a bit for every additional passive it has.</t>
+  </si>
+  <si>
+    <t>That's why a Dagger helps you move faster but hits not-as-hard.</t>
+  </si>
+  <si>
+    <t>Or an Axe hits very hard but isn't as accurate.</t>
+  </si>
+  <si>
+    <t>Different weapon types have different built-in passives.</t>
+  </si>
+  <si>
+    <t>That kind of thing.</t>
+  </si>
+  <si>
+    <t>So…</t>
+  </si>
+  <si>
+    <t>WEAPON NAME</t>
+  </si>
+  <si>
+    <t>Type (Sword, Dagger, Etc.)</t>
+  </si>
+  <si>
+    <t>Rarity</t>
+  </si>
+  <si>
+    <t>Attack Power</t>
+  </si>
+  <si>
+    <t>Additional Passives and Effects</t>
+  </si>
+  <si>
+    <t>Cost</t>
+  </si>
+  <si>
+    <t>Icon</t>
+  </si>
+  <si>
+    <t>Color Information</t>
+  </si>
 </sst>
 </file>
 
@@ -292,7 +353,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -447,7 +508,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -469,17 +530,20 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="4" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="4" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="165" fontId="0" fillId="5" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="165" fontId="0" fillId="6" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="4" fillId="7" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="4" fillId="7" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="4" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -524,7 +588,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E1A01606-F80E-4EA2-98BA-7659994D9D51}" name="Table1" displayName="Table1" ref="A1:E7" totalsRowCount="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E1A01606-F80E-4EA2-98BA-7659994D9D51}" name="ArchetypeGrowths" displayName="ArchetypeGrowths" ref="A1:E7" totalsRowCount="1">
   <autoFilter ref="A1:E6" xr:uid="{E1A01606-F80E-4EA2-98BA-7659994D9D51}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{486137BA-44D5-40FB-89BE-88D888F85C59}" name="ARCHETYPE" totalsRowLabel="Total"/>
@@ -1698,6 +1762,111 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AFC06FF6-5183-478B-AB66-71586CA9F359}">
+  <dimension ref="D2:D22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="3" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="4" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D4" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="6" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D6" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="8" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D8" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="9" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D9" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="10" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D10" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="11" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D11" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="13" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D13" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="14" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D14" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="15" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D15" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="16" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D16" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="17" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D17" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D18" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="19" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D19" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="20" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D20" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="21" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D21" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="22" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D22" t="s">
+        <v>98</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8F8B701-6211-4913-A6E5-62A20A5B14C8}">
   <dimension ref="B5:S41"/>
@@ -8425,7 +8594,7 @@
   <dimension ref="A1:U114"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="R6" sqref="R6"/>
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13958,8 +14127,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5234A45-9045-4438-9498-5D3A4A622F57}">
   <dimension ref="C3:L64"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F37" sqref="F37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14267,19 +14436,19 @@
         <v>2</v>
       </c>
       <c r="G36" s="21">
-        <f>ROUND(($D$40*$C$37^$D$37)+($D$46*F36^$D$43),0)</f>
+        <f t="shared" ref="G36:G46" si="1">ROUND(($D$40*$C$37^$D$37)+($D$46*F36^$D$43),0)</f>
         <v>37</v>
       </c>
       <c r="I36">
-        <f>ROUNDDOWN($G36/I$35,1)</f>
+        <f t="shared" ref="I36:K46" si="2">ROUNDDOWN($G36/I$35,1)</f>
         <v>3.7</v>
       </c>
       <c r="J36">
-        <f>ROUNDDOWN($G36/J$35,1)</f>
+        <f t="shared" si="2"/>
         <v>1.2</v>
       </c>
       <c r="K36">
-        <f>ROUNDDOWN($G36/K$35,1)</f>
+        <f t="shared" si="2"/>
         <v>0.6</v>
       </c>
     </row>
@@ -14298,19 +14467,19 @@
         <v>3</v>
       </c>
       <c r="G37" s="21">
-        <f>ROUND(($D$40*$C$37^$D$37)+($D$46*F37^$D$43),0)</f>
+        <f t="shared" si="1"/>
         <v>48</v>
       </c>
       <c r="I37">
-        <f>ROUNDDOWN($G37/I$35,1)</f>
+        <f t="shared" si="2"/>
         <v>4.8</v>
       </c>
       <c r="J37">
-        <f>ROUNDDOWN($G37/J$35,1)</f>
+        <f t="shared" si="2"/>
         <v>1.6</v>
       </c>
       <c r="K37">
-        <f>ROUNDDOWN($G37/K$35,1)</f>
+        <f t="shared" si="2"/>
         <v>0.8</v>
       </c>
     </row>
@@ -14325,19 +14494,19 @@
         <v>4</v>
       </c>
       <c r="G38" s="19">
-        <f>ROUND(($D$40*$C$37^$D$37)+($D$46*F38^$D$43),0)</f>
+        <f t="shared" si="1"/>
         <v>61</v>
       </c>
       <c r="I38">
-        <f>ROUNDDOWN($G38/I$35,1)</f>
+        <f t="shared" si="2"/>
         <v>6.1</v>
       </c>
       <c r="J38">
-        <f>ROUNDDOWN($G38/J$35,1)</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="K38">
-        <f>ROUNDDOWN($G38/K$35,1)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -14356,19 +14525,19 @@
         <v>6</v>
       </c>
       <c r="G39" s="19">
-        <f>ROUND(($D$40*$C$37^$D$37)+($D$46*F39^$D$43),0)</f>
+        <f t="shared" si="1"/>
         <v>90</v>
       </c>
       <c r="I39">
-        <f>ROUNDDOWN($G39/I$35,1)</f>
+        <f t="shared" si="2"/>
         <v>9</v>
       </c>
       <c r="J39">
-        <f>ROUNDDOWN($G39/J$35,1)</f>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="K39">
-        <f>ROUNDDOWN($G39/K$35,1)</f>
+        <f t="shared" si="2"/>
         <v>1.5</v>
       </c>
     </row>
@@ -14387,19 +14556,19 @@
         <v>7</v>
       </c>
       <c r="G40" s="17">
-        <f>ROUND(($D$40*$C$37^$D$37)+($D$46*F40^$D$43),0)</f>
+        <f t="shared" si="1"/>
         <v>106</v>
       </c>
       <c r="I40">
-        <f>ROUNDDOWN($G40/I$35,1)</f>
+        <f t="shared" si="2"/>
         <v>10.6</v>
       </c>
       <c r="J40">
-        <f>ROUNDDOWN($G40/J$35,1)</f>
+        <f t="shared" si="2"/>
         <v>3.5</v>
       </c>
       <c r="K40">
-        <f>ROUNDDOWN($G40/K$35,1)</f>
+        <f t="shared" si="2"/>
         <v>1.7</v>
       </c>
     </row>
@@ -14413,19 +14582,19 @@
         <v>8</v>
       </c>
       <c r="G41" s="17">
-        <f>ROUND(($D$40*$C$37^$D$37)+($D$46*F41^$D$43),0)</f>
+        <f t="shared" si="1"/>
         <v>122</v>
       </c>
       <c r="I41">
-        <f>ROUNDDOWN($G41/I$35,1)</f>
+        <f t="shared" si="2"/>
         <v>12.2</v>
       </c>
       <c r="J41">
-        <f>ROUNDDOWN($G41/J$35,1)</f>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="K41">
-        <f>ROUNDDOWN($G41/K$35,1)</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
     </row>
@@ -14441,19 +14610,19 @@
         <v>9</v>
       </c>
       <c r="G42" s="15">
-        <f>ROUND(($D$40*$C$37^$D$37)+($D$46*F42^$D$43),0)</f>
+        <f t="shared" si="1"/>
         <v>139</v>
       </c>
       <c r="I42">
-        <f>ROUNDDOWN($G42/I$35,1)</f>
+        <f t="shared" si="2"/>
         <v>13.9</v>
       </c>
       <c r="J42">
-        <f>ROUNDDOWN($G42/J$35,1)</f>
+        <f t="shared" si="2"/>
         <v>4.5999999999999996</v>
       </c>
       <c r="K42">
-        <f>ROUNDDOWN($G42/K$35,1)</f>
+        <f t="shared" si="2"/>
         <v>2.2999999999999998</v>
       </c>
     </row>
@@ -14469,19 +14638,19 @@
         <v>10</v>
       </c>
       <c r="G43" s="15">
-        <f>ROUND(($D$40*$C$37^$D$37)+($D$46*F43^$D$43),0)</f>
+        <f t="shared" si="1"/>
         <v>157</v>
       </c>
       <c r="I43">
-        <f>ROUNDDOWN($G43/I$35,1)</f>
+        <f t="shared" si="2"/>
         <v>15.7</v>
       </c>
       <c r="J43">
-        <f>ROUNDDOWN($G43/J$35,1)</f>
+        <f t="shared" si="2"/>
         <v>5.2</v>
       </c>
       <c r="K43">
-        <f>ROUNDDOWN($G43/K$35,1)</f>
+        <f t="shared" si="2"/>
         <v>2.6</v>
       </c>
     </row>
@@ -14495,19 +14664,19 @@
         <v>11</v>
       </c>
       <c r="G44" s="13">
-        <f>ROUND(($D$40*$C$37^$D$37)+($D$46*F44^$D$43),0)</f>
+        <f t="shared" si="1"/>
         <v>175</v>
       </c>
       <c r="I44">
-        <f>ROUNDDOWN($G44/I$35,1)</f>
+        <f t="shared" si="2"/>
         <v>17.5</v>
       </c>
       <c r="J44">
-        <f>ROUNDDOWN($G44/J$35,1)</f>
+        <f t="shared" si="2"/>
         <v>5.8</v>
       </c>
       <c r="K44">
-        <f>ROUNDDOWN($G44/K$35,1)</f>
+        <f t="shared" si="2"/>
         <v>2.9</v>
       </c>
     </row>
@@ -14523,19 +14692,19 @@
         <v>12</v>
       </c>
       <c r="G45" s="13">
-        <f>ROUND(($D$40*$C$37^$D$37)+($D$46*F45^$D$43),0)</f>
+        <f t="shared" si="1"/>
         <v>193</v>
       </c>
       <c r="I45">
-        <f>ROUNDDOWN($G45/I$35,1)</f>
+        <f t="shared" si="2"/>
         <v>19.3</v>
       </c>
       <c r="J45">
-        <f>ROUNDDOWN($G45/J$35,1)</f>
+        <f t="shared" si="2"/>
         <v>6.4</v>
       </c>
       <c r="K45">
-        <f>ROUNDDOWN($G45/K$35,1)</f>
+        <f t="shared" si="2"/>
         <v>3.2</v>
       </c>
     </row>
@@ -14551,19 +14720,19 @@
         <v>13</v>
       </c>
       <c r="G46" s="11">
-        <f>ROUND(($D$40*$C$37^$D$37)+($D$46*F46^$D$43),0)</f>
+        <f t="shared" si="1"/>
         <v>213</v>
       </c>
       <c r="I46">
-        <f>ROUNDDOWN($G46/I$35,1)</f>
+        <f t="shared" si="2"/>
         <v>21.3</v>
       </c>
       <c r="J46">
-        <f>ROUNDDOWN($G46/J$35,1)</f>
+        <f t="shared" si="2"/>
         <v>7.1</v>
       </c>
       <c r="K46">
-        <f>ROUNDDOWN($G46/K$35,1)</f>
+        <f t="shared" si="2"/>
         <v>3.5</v>
       </c>
     </row>
@@ -14623,7 +14792,7 @@
         <v>2</v>
       </c>
       <c r="G54" s="21">
-        <f>ROUND(($D$58*$C$55^$D$55)+($D$64*F54^$D$61),0)</f>
+        <f t="shared" ref="G54:G64" si="3">ROUND(($D$58*$C$55^$D$55)+($D$64*F54^$D$61),0)</f>
         <v>8</v>
       </c>
       <c r="I54">
@@ -14631,11 +14800,11 @@
         <v>1.6</v>
       </c>
       <c r="J54">
-        <f t="shared" ref="J54:K54" si="1">ROUNDDOWN($G54/J$53,1)</f>
+        <f t="shared" ref="J54:K54" si="4">ROUNDDOWN($G54/J$53,1)</f>
         <v>0.4</v>
       </c>
       <c r="K54">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0.1</v>
       </c>
     </row>
@@ -14654,19 +14823,19 @@
         <v>3</v>
       </c>
       <c r="G55" s="21">
-        <f>ROUND(($D$58*$C$55^$D$55)+($D$64*F55^$D$61),0)</f>
+        <f t="shared" si="3"/>
         <v>10</v>
       </c>
       <c r="I55">
-        <f t="shared" ref="I55:K64" si="2">ROUNDDOWN($G55/I$53,1)</f>
+        <f t="shared" ref="I55:K64" si="5">ROUNDDOWN($G55/I$53,1)</f>
         <v>2</v>
       </c>
       <c r="J55">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0.5</v>
       </c>
       <c r="K55">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0.2</v>
       </c>
     </row>
@@ -14681,19 +14850,19 @@
         <v>4</v>
       </c>
       <c r="G56" s="19">
-        <f>ROUND(($D$58*$C$55^$D$55)+($D$64*F56^$D$61),0)</f>
+        <f t="shared" si="3"/>
         <v>13</v>
       </c>
       <c r="I56">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>2.6</v>
       </c>
       <c r="J56">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0.6</v>
       </c>
       <c r="K56">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0.2</v>
       </c>
     </row>
@@ -14712,19 +14881,19 @@
         <v>6</v>
       </c>
       <c r="G57" s="19">
-        <f>ROUND(($D$58*$C$55^$D$55)+($D$64*F57^$D$61),0)</f>
+        <f t="shared" si="3"/>
         <v>18</v>
       </c>
       <c r="I57">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>3.6</v>
       </c>
       <c r="J57">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0.9</v>
       </c>
       <c r="K57">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0.3</v>
       </c>
     </row>
@@ -14743,19 +14912,19 @@
         <v>7</v>
       </c>
       <c r="G58" s="17">
-        <f>ROUND(($D$58*$C$55^$D$55)+($D$64*F58^$D$61),0)</f>
+        <f t="shared" si="3"/>
         <v>20</v>
       </c>
       <c r="I58">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>4</v>
       </c>
       <c r="J58">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="K58">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0.4</v>
       </c>
     </row>
@@ -14769,19 +14938,19 @@
         <v>8</v>
       </c>
       <c r="G59" s="17">
-        <f>ROUND(($D$58*$C$55^$D$55)+($D$64*F59^$D$61),0)</f>
+        <f t="shared" si="3"/>
         <v>23</v>
       </c>
       <c r="I59">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>4.5999999999999996</v>
       </c>
       <c r="J59">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1.1000000000000001</v>
       </c>
       <c r="K59">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0.4</v>
       </c>
     </row>
@@ -14797,19 +14966,19 @@
         <v>9</v>
       </c>
       <c r="G60" s="15">
-        <f>ROUND(($D$58*$C$55^$D$55)+($D$64*F60^$D$61),0)</f>
+        <f t="shared" si="3"/>
         <v>26</v>
       </c>
       <c r="I60">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>5.2</v>
       </c>
       <c r="J60">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1.3</v>
       </c>
       <c r="K60">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0.5</v>
       </c>
     </row>
@@ -14825,19 +14994,19 @@
         <v>10</v>
       </c>
       <c r="G61" s="15">
-        <f>ROUND(($D$58*$C$55^$D$55)+($D$64*F61^$D$61),0)</f>
+        <f t="shared" si="3"/>
         <v>29</v>
       </c>
       <c r="I61">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>5.8</v>
       </c>
       <c r="J61">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1.4</v>
       </c>
       <c r="K61">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0.5</v>
       </c>
     </row>
@@ -14851,19 +15020,19 @@
         <v>11</v>
       </c>
       <c r="G62" s="13">
-        <f>ROUND(($D$58*$C$55^$D$55)+($D$64*F62^$D$61),0)</f>
+        <f t="shared" si="3"/>
         <v>31</v>
       </c>
       <c r="I62">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>6.2</v>
       </c>
       <c r="J62">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1.5</v>
       </c>
       <c r="K62">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0.6</v>
       </c>
     </row>
@@ -14879,19 +15048,19 @@
         <v>12</v>
       </c>
       <c r="G63" s="13">
-        <f>ROUND(($D$58*$C$55^$D$55)+($D$64*F63^$D$61),0)</f>
+        <f t="shared" si="3"/>
         <v>34</v>
       </c>
       <c r="I63">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>6.8</v>
       </c>
       <c r="J63">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1.7</v>
       </c>
       <c r="K63">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0.6</v>
       </c>
     </row>
@@ -14907,19 +15076,19 @@
         <v>13</v>
       </c>
       <c r="G64" s="11">
-        <f>ROUND(($D$58*$C$55^$D$55)+($D$64*F64^$D$61),0)</f>
+        <f t="shared" si="3"/>
         <v>37</v>
       </c>
       <c r="I64">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>7.4</v>
       </c>
       <c r="J64">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>1.8</v>
       </c>
       <c r="K64">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>0.7</v>
       </c>
     </row>
@@ -14934,16 +15103,21 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F82EB0E4-D9D7-4D2E-96C4-1C88BE71FF97}">
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:I22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.42578125" customWidth="1"/>
     <col min="2" max="2" width="10.7109375" customWidth="1"/>
+    <col min="5" max="5" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -15068,24 +15242,152 @@
         <v>52</v>
       </c>
       <c r="B7">
-        <f>SUBTOTAL(109,Table1[Barbarian])</f>
+        <f>SUBTOTAL(109,ArchetypeGrowths[Barbarian])</f>
         <v>6.5</v>
       </c>
       <c r="C7">
-        <f>SUBTOTAL(109,Table1[Fighter])</f>
+        <f>SUBTOTAL(109,ArchetypeGrowths[Fighter])</f>
         <v>6.5</v>
       </c>
       <c r="D7">
-        <f>SUBTOTAL(109,Table1[Black Mage])</f>
+        <f>SUBTOTAL(109,ArchetypeGrowths[Black Mage])</f>
         <v>6.5</v>
       </c>
       <c r="E7">
-        <f>SUBTOTAL(109,Table1[White Mage])</f>
+        <f>SUBTOTAL(109,ArchetypeGrowths[White Mage])</f>
         <v>6.5</v>
       </c>
       <c r="H7">
         <f>SUM(H2:H6)</f>
         <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D17" t="s">
+        <v>14</v>
+      </c>
+      <c r="E17" t="s">
+        <v>79</v>
+      </c>
+      <c r="F17" t="s">
+        <v>78</v>
+      </c>
+      <c r="G17" t="s">
+        <v>53</v>
+      </c>
+      <c r="H17" s="22" t="s">
+        <v>80</v>
+      </c>
+      <c r="I17" s="22" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="18" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D18">
+        <v>10</v>
+      </c>
+      <c r="E18" t="s">
+        <v>16</v>
+      </c>
+      <c r="F18">
+        <f>INDEX(A2:E2,1,MATCH($F$17,ArchetypeGrowths[#Headers],0))</f>
+        <v>1</v>
+      </c>
+      <c r="G18">
+        <f>INDEX(A2:E2,1,MATCH($G$17,ArchetypeGrowths[#Headers],0))</f>
+        <v>1</v>
+      </c>
+      <c r="H18" s="22">
+        <f>SUM(F18:G18)</f>
+        <v>2</v>
+      </c>
+      <c r="I18" s="22">
+        <f>VLOOKUP($D$18,'Stat Progression &amp; Growth Rates'!$F$4:$Q$103,MATCH(H18,'Stat Progression &amp; Growth Rates'!$F$3:$Q$3,0))</f>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="19" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="E19" t="s">
+        <v>20</v>
+      </c>
+      <c r="F19">
+        <f>INDEX(A3:E3,1,MATCH($F$17,ArchetypeGrowths[#Headers],0))</f>
+        <v>1.5</v>
+      </c>
+      <c r="G19">
+        <f>INDEX(A3:E3,1,MATCH($G$17,ArchetypeGrowths[#Headers],0))</f>
+        <v>0.5</v>
+      </c>
+      <c r="H19" s="22">
+        <f t="shared" ref="H19:H22" si="0">SUM(F19:G19)</f>
+        <v>2</v>
+      </c>
+      <c r="I19" s="22">
+        <f>VLOOKUP($D$18,'Stat Progression &amp; Growth Rates'!$F$4:$Q$103,MATCH(H19,'Stat Progression &amp; Growth Rates'!$F$3:$Q$3,0))</f>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="20" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="E20" t="s">
+        <v>24</v>
+      </c>
+      <c r="F20">
+        <f>INDEX(A4:E4,1,MATCH($F$17,ArchetypeGrowths[#Headers],0))</f>
+        <v>1</v>
+      </c>
+      <c r="G20">
+        <f>INDEX(A4:E4,1,MATCH($G$17,ArchetypeGrowths[#Headers],0))</f>
+        <v>2</v>
+      </c>
+      <c r="H20" s="22">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="I20" s="22">
+        <f>VLOOKUP($D$18,'Stat Progression &amp; Growth Rates'!$F$4:$Q$103,MATCH(H20,'Stat Progression &amp; Growth Rates'!$F$3:$Q$3,0))</f>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="E21" t="s">
+        <v>25</v>
+      </c>
+      <c r="F21">
+        <f>INDEX(A5:E5,1,MATCH($F$17,ArchetypeGrowths[#Headers],0))</f>
+        <v>1</v>
+      </c>
+      <c r="G21">
+        <f>INDEX(A5:E5,1,MATCH($G$17,ArchetypeGrowths[#Headers],0))</f>
+        <v>2</v>
+      </c>
+      <c r="H21" s="22">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="I21" s="22">
+        <f>VLOOKUP($D$18,'Stat Progression &amp; Growth Rates'!$F$4:$Q$103,MATCH(H21,'Stat Progression &amp; Growth Rates'!$F$3:$Q$3,0))</f>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="22" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="E22" t="s">
+        <v>26</v>
+      </c>
+      <c r="F22">
+        <f>INDEX(A6:E6,1,MATCH($F$17,ArchetypeGrowths[#Headers],0))</f>
+        <v>2</v>
+      </c>
+      <c r="G22">
+        <f>INDEX(A6:E6,1,MATCH($G$17,ArchetypeGrowths[#Headers],0))</f>
+        <v>1</v>
+      </c>
+      <c r="H22" s="22">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="I22" s="22">
+        <f>VLOOKUP($D$18,'Stat Progression &amp; Growth Rates'!$F$4:$Q$103,MATCH(H22,'Stat Progression &amp; Growth Rates'!$F$3:$Q$3,0))</f>
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>